<commit_message>
ejecución exitosa hu06 p7 res
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/automation.xlsx
+++ b/src/test/resources/configs/automation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mortegabuitr\eclipse-workspace\payment_collector\src\test\resources\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726370CC-B60A-470F-B645-AA6291EE3F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80AD820-A55D-4CE3-8F0C-E96CA7404696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{A04BB19C-3AAB-4633-A5CA-B8709A517DBD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="46">
   <si>
     <t>Reserva</t>
   </si>
@@ -132,13 +132,58 @@
   </si>
   <si>
     <t>Reserva no contiene un itinerario confirmado</t>
+  </si>
+  <si>
+    <t>4NH735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4NHRS5 </t>
+  </si>
+  <si>
+    <t>4NJFSO</t>
+  </si>
+  <si>
+    <t>4NFLE3</t>
+  </si>
+  <si>
+    <t>4NKXIZ</t>
+  </si>
+  <si>
+    <t>4NGLGR</t>
+  </si>
+  <si>
+    <t>4MT8WU</t>
+  </si>
+  <si>
+    <t>Reserva sin Nombre completo en el Apis/TSA</t>
+  </si>
+  <si>
+    <t>Reserva sin  fecha de nacimiento en el Apis/TSA</t>
+  </si>
+  <si>
+    <t>Reserva sin Genero en el Apis/TSA</t>
+  </si>
+  <si>
+    <t>Reserva sin  Numero de documento en el Apis/TSA</t>
+  </si>
+  <si>
+    <t>Reserva sin nacionalidad en el Apis/TSA</t>
+  </si>
+  <si>
+    <t>Los itinerarios que contengan ciudades de los siguientes países en sus segmentos de vuelo origen o destino: Estados unidos</t>
+  </si>
+  <si>
+    <t>Los itinerarios que contengan ciudades de los siguientes países en sus segmentos de vuelo origen o destino: Canadá</t>
+  </si>
+  <si>
+    <t>Por favor ingrese el APIS/TSA en la reserva</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,8 +213,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,8 +275,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -262,11 +343,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -311,6 +437,36 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -638,7 +794,7 @@
       <selection activeCell="D6" sqref="A6:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="39.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="39.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12.6328125" customWidth="1"/>
     <col min="2" max="2" width="40.26953125" customWidth="1"/>
@@ -646,7 +802,7 @@
     <col min="4" max="4" width="23.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="17" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -660,7 +816,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="39.5" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -674,7 +830,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="39.5" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -686,7 +842,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="39.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -700,7 +856,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="39.5" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>25</v>
       </c>
@@ -712,7 +868,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="39.5" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -726,7 +882,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="39.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -756,14 +912,14 @@
       <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="23.54296875" customWidth="1"/>
     <col min="3" max="3" width="14.453125" customWidth="1"/>
     <col min="4" max="4" width="29.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -777,7 +933,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="58" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
@@ -791,7 +947,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="89.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="89.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -819,14 +975,14 @@
       <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="35.81640625" customWidth="1"/>
     <col min="3" max="3" width="16.90625" customWidth="1"/>
     <col min="4" max="4" width="29.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -840,7 +996,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="42" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -854,7 +1010,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="74" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="74" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -866,7 +1022,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="61.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -880,7 +1036,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="67.5" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>25</v>
       </c>
@@ -892,7 +1048,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="77.5" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -906,7 +1062,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="48" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -918,7 +1074,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="82.5" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
@@ -932,7 +1088,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="47.5" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -944,7 +1100,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="59.5" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>27</v>
       </c>
@@ -958,7 +1114,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="58">
       <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
@@ -972,7 +1128,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="29">
       <c r="A12" s="6" t="s">
         <v>22</v>
       </c>
@@ -999,21 +1155,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{573BE517-630B-4674-8992-44A924E9EB8C}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" customWidth="1"/>
     <col min="2" max="2" width="23.26953125" customWidth="1"/>
     <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15" thickBot="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1027,62 +1183,96 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
+    <row r="2" spans="1:4" ht="29">
+      <c r="A2" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
+      <c r="D2" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="29">
+      <c r="A3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>39</v>
       </c>
       <c r="C3" s="11"/>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
+      <c r="D3" s="24"/>
+    </row>
+    <row r="4" spans="1:4" ht="29">
+      <c r="A4" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>40</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
+      <c r="D4" s="24"/>
+    </row>
+    <row r="5" spans="1:4" ht="29">
+      <c r="A5" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>41</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="D5" s="24"/>
+    </row>
+    <row r="6" spans="1:4" ht="29">
+      <c r="A6" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="24"/>
+    </row>
+    <row r="7" spans="1:4" ht="87">
+      <c r="A7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="24"/>
+    </row>
+    <row r="8" spans="1:4" ht="72.5">
+      <c r="A8" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="24"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="D9" s="24"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="D10" s="24"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="D11" s="24"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="D12" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D2:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>